<commit_message>
update to QT HEWR
</commit_message>
<xml_diff>
--- a/data/QT/Count_summary_QT_HEWR.xlsx
+++ b/data/QT/Count_summary_QT_HEWR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clayton.lamb/Google Drive/Documents/University/PDF/PDF Analyses/KZdemography/KZ_QT_IPM/data/QT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B16241C-FBC1-6042-995F-1E8D7BF00DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EDAC70-B025-B94D-A228-A942BB998E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="500" windowWidth="28720" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33220" yWindow="1820" windowWidth="28720" windowHeight="15380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MinCount_summary_KZ-withimm" sheetId="2" r:id="rId1"/>
@@ -101,9 +101,6 @@
     <t>MinCount_CALFMF</t>
   </si>
   <si>
-    <t>##not finalized, new data, check with Agnes</t>
-  </si>
-  <si>
     <t>Estimate</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>Slight difference from the report due to removal of one group of 2 caribou (with one collar) that was outside the herd range . Data Update: 2016 report records 'juveniles = 6', updated to 'juveniles = 5', one group of two caribou (one collared, car 191) determined to be outside herd boundary. Report has sightability at 7/15, but two animals not within HEWR, so to get HEWR sightability we use 7/13</t>
+  </si>
+  <si>
+    <t>Pelletier 2021 In prep</t>
   </si>
 </sst>
 </file>
@@ -986,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1014,7 +1014,7 @@
         <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
         <v>21</v>
@@ -1050,7 +1050,7 @@
         <v>11</v>
       </c>
       <c r="O1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P1" t="s">
         <v>1</v>
@@ -1062,7 +1062,7 @@
         <v>6</v>
       </c>
       <c r="S1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -1134,7 +1134,7 @@
         <v>17</v>
       </c>
       <c r="S3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -1235,7 +1235,7 @@
         <v>7</v>
       </c>
       <c r="S9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -1280,10 +1280,10 @@
       </c>
       <c r="C14">
         <f>SUM(D14:E14)</f>
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D14">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E14">
         <v>9</v>
@@ -1327,10 +1327,10 @@
         <v>12</v>
       </c>
       <c r="Q14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
@@ -1355,7 +1355,7 @@
       </c>
       <c r="B17">
         <f>G17+F17</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <f>SUM(D17:E17)</f>
@@ -1368,7 +1368,7 @@
         <v>7</v>
       </c>
       <c r="F17">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G17">
         <v>5</v>
@@ -1377,39 +1377,39 @@
         <v>0.64</v>
       </c>
       <c r="I17">
-        <v>0.54</v>
+        <v>0.7</v>
       </c>
       <c r="J17">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="K17">
         <f>F17/I17</f>
-        <v>40.74074074074074</v>
+        <v>34.285714285714285</v>
       </c>
       <c r="L17">
         <f>F17*J17</f>
-        <v>3.08</v>
+        <v>3.5999999999999996</v>
       </c>
       <c r="M17">
         <f>G17/I17</f>
-        <v>9.2592592592592595</v>
+        <v>7.1428571428571432</v>
       </c>
       <c r="N17">
         <f>G17*J17</f>
-        <v>0.70000000000000007</v>
+        <v>0.75</v>
       </c>
       <c r="O17">
         <f>SUM(M17,K17)</f>
-        <v>50</v>
+        <v>41.428571428571431</v>
       </c>
       <c r="P17" t="s">
         <v>18</v>
       </c>
       <c r="Q17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
@@ -1477,10 +1477,10 @@
         <v>19</v>
       </c>
       <c r="Q19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
@@ -1493,13 +1493,13 @@
       </c>
       <c r="C20">
         <f>SUM(D20:E20)</f>
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="D20" s="2">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="E20">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F20" s="2">
         <v>36</v>
@@ -1540,10 +1540,10 @@
         <v>20</v>
       </c>
       <c r="Q20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
@@ -1564,13 +1564,13 @@
       </c>
       <c r="C22">
         <f>SUM(D22:E22)</f>
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="D22">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="E22">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>39</v>
@@ -1592,11 +1592,11 @@
         <v>78</v>
       </c>
       <c r="L22">
-        <f t="shared" ref="L22" si="0">F22*J22</f>
+        <f>F22*J22</f>
         <v>6.6300000000000008</v>
       </c>
       <c r="M22">
-        <f t="shared" ref="M22" si="1">G22/I22</f>
+        <f>G22/I22</f>
         <v>20</v>
       </c>
       <c r="N22">
@@ -1608,10 +1608,10 @@
         <v>98</v>
       </c>
       <c r="P22" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="S22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>